<commit_message>
Updated schema, json and yaml files
</commit_message>
<xml_diff>
--- a/single_cell/singlecell_schema_main_v0.4.xlsx
+++ b/single_cell/singlecell_schema_main_v0.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/providen/Documents/EI/Projects/COPO-schemas/single_cell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3428CF79-5F0C-7249-908E-17DAFB5DC95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1598FD3A-249D-A64B-84A0-80E44C22A543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18000" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" activeTab="5" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3140" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3144" uniqueCount="1267">
   <si>
     <t>component_name</t>
   </si>
@@ -4008,6 +4008,12 @@
   </si>
   <si>
     <t>Expected text with no leading or trailing spaces, followed by a space and a tag in the format Letters:Numbers.</t>
+  </si>
+  <si>
+    <t>AND(LEN(({column_letter}{row_start})-LEN(SUBSTITUTE(({column_letter}{row_start},":",""))=1,   LEN(({column_letter}{row_start})-LEN(SUBSTITUTE(LEFT(({column_letter}{row_start},FIND(":",({column_letter}{row_start})-1),"A",""))&gt;0,  LEN(LEFT(({column_letter}{row_start},FIND(":",({column_letter}{row_start})-1))&gt;=2,   ISNUMBER(VALUE(RIGHT(({column_letter}{row_start},LEN(({column_letter}{row_start})-FIND(":",({column_letter}{row_start})))))</t>
+  </si>
+  <si>
+    <t>AND( LEN(({column_letter}{row_start})=32, LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTESUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(({column_letter}{row_start},"0",""),"1",""),"2",""),"3",""),"4",""),"5",""), "6",""),"7",""),"8",""),"9",""),"a",""),"b",""),"c",""),"d",""),"e",""),"f","") )=0)</t>
   </si>
 </sst>
 </file>
@@ -5374,7 +5380,7 @@
   </sheetPr>
   <dimension ref="A1:S203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="A23" sqref="A23"/>
       <selection pane="topRight" activeCell="L9" sqref="L9"/>
@@ -26569,10 +26575,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27160,7 +27166,7 @@
       </c>
       <c r="C58" s="27"/>
     </row>
-    <row r="59" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="49" t="s">
         <v>163</v>
       </c>
@@ -27177,6 +27183,24 @@
         <v>1205</v>
       </c>
       <c r="C60" s="50"/>
+    </row>
+    <row r="61" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="49" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B61" s="49" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C61" s="50"/>
+    </row>
+    <row r="62" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="49" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B62" s="49" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C62" s="50"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C53" xr:uid="{D95B3E19-31EE-401E-8E14-DBEF7BC74F95}"/>
@@ -27192,7 +27216,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>